<commit_message>
added nfc connector + update pinout info
</commit_message>
<xml_diff>
--- a/Pinout.xlsx
+++ b/Pinout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nico\Desktop\PSoM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n.degrave\Desktop\PSoM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3AE687-F5BF-4937-BE07-86280B888081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4735A5CA-5BA3-4795-B38C-F1F24A7656D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="8070" windowHeight="17010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14745" yWindow="-20700" windowWidth="25770" windowHeight="20685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="124">
   <si>
     <t>Pins</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Battery temp</t>
   </si>
   <si>
-    <t>Fixed pins</t>
-  </si>
-  <si>
     <t>ESP32S2</t>
   </si>
   <si>
@@ -199,6 +196,207 @@
   </si>
   <si>
     <t>SCL2</t>
+  </si>
+  <si>
+    <t>nRF52840</t>
+  </si>
+  <si>
+    <t>P0.06</t>
+  </si>
+  <si>
+    <t>P0.07</t>
+  </si>
+  <si>
+    <t>P0.08</t>
+  </si>
+  <si>
+    <t>P1.08</t>
+  </si>
+  <si>
+    <t>P0.00</t>
+  </si>
+  <si>
+    <t>P0.01</t>
+  </si>
+  <si>
+    <t>P0.30</t>
+  </si>
+  <si>
+    <t>P0.04</t>
+  </si>
+  <si>
+    <t>P0.05</t>
+  </si>
+  <si>
+    <t>P1.10</t>
+  </si>
+  <si>
+    <t>P0.29</t>
+  </si>
+  <si>
+    <t>P0.31</t>
+  </si>
+  <si>
+    <t>P1.13</t>
+  </si>
+  <si>
+    <t>P1.04</t>
+  </si>
+  <si>
+    <t>P1.15</t>
+  </si>
+  <si>
+    <t>P1.09</t>
+  </si>
+  <si>
+    <t>P0.21</t>
+  </si>
+  <si>
+    <t>P0.23</t>
+  </si>
+  <si>
+    <t>P0.18</t>
+  </si>
+  <si>
+    <t>P0.20</t>
+  </si>
+  <si>
+    <t>P0.19</t>
+  </si>
+  <si>
+    <t>P0.22</t>
+  </si>
+  <si>
+    <t>P0.26</t>
+  </si>
+  <si>
+    <t>P0.27</t>
+  </si>
+  <si>
+    <t>P0.14</t>
+  </si>
+  <si>
+    <t>P0.15</t>
+  </si>
+  <si>
+    <t>P0.16</t>
+  </si>
+  <si>
+    <t>P0.17</t>
+  </si>
+  <si>
+    <t>P0.24</t>
+  </si>
+  <si>
+    <t>P0.25</t>
+  </si>
+  <si>
+    <t>P1.01</t>
+  </si>
+  <si>
+    <t>SDWCLK</t>
+  </si>
+  <si>
+    <t>SDWDIO</t>
+  </si>
+  <si>
+    <t>P1.02</t>
+  </si>
+  <si>
+    <t>P1.00</t>
+  </si>
+  <si>
+    <t>P0.11</t>
+  </si>
+  <si>
+    <t>P0.12</t>
+  </si>
+  <si>
+    <t>IO2</t>
+  </si>
+  <si>
+    <t>IO3</t>
+  </si>
+  <si>
+    <t>IO18</t>
+  </si>
+  <si>
+    <t>IO21</t>
+  </si>
+  <si>
+    <t>IO4</t>
+  </si>
+  <si>
+    <t>IO5</t>
+  </si>
+  <si>
+    <t>IO6</t>
+  </si>
+  <si>
+    <t>IO7</t>
+  </si>
+  <si>
+    <t>IO8</t>
+  </si>
+  <si>
+    <t>IO9</t>
+  </si>
+  <si>
+    <t>IO10</t>
+  </si>
+  <si>
+    <t>IO11</t>
+  </si>
+  <si>
+    <t>IO12</t>
+  </si>
+  <si>
+    <t>IO13</t>
+  </si>
+  <si>
+    <t>IO14</t>
+  </si>
+  <si>
+    <t>IO15</t>
+  </si>
+  <si>
+    <t>IO16</t>
+  </si>
+  <si>
+    <t>IO17</t>
+  </si>
+  <si>
+    <t>IO0</t>
+  </si>
+  <si>
+    <t>IO34</t>
+  </si>
+  <si>
+    <t>IO35</t>
+  </si>
+  <si>
+    <t>IO33</t>
+  </si>
+  <si>
+    <t>IO36</t>
+  </si>
+  <si>
+    <t>IO37</t>
+  </si>
+  <si>
+    <t>IO38</t>
+  </si>
+  <si>
+    <t>IO41</t>
+  </si>
+  <si>
+    <t>IO39</t>
+  </si>
+  <si>
+    <t>IO40</t>
+  </si>
+  <si>
+    <t>IO42</t>
   </si>
 </sst>
 </file>
@@ -507,7 +705,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -531,37 +729,27 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -570,41 +758,48 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -888,18 +1083,20 @@
   <dimension ref="A1:W64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
@@ -908,83 +1105,87 @@
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" s="8" t="s">
+      <c r="M1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="23" t="s">
+    </row>
+    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="36"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+    </row>
+    <row r="4" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="47" t="s">
+      <c r="E4" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="H4" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="48" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="50" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="J4" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="55" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>1</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="13">
+      <c r="C5" s="29"/>
+      <c r="G5" s="13">
         <v>2</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="H5" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="25"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="I5" s="38"/>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
@@ -1000,24 +1201,21 @@
       <c r="V5" s="12"/>
       <c r="W5" s="12"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>3</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="13">
+      <c r="C6" s="31"/>
+      <c r="G6" s="13">
         <v>4</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="H6" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
+      <c r="I6" s="40"/>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
@@ -1033,300 +1231,463 @@
       <c r="V6" s="12"/>
       <c r="W6" s="12"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>5</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="13">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="13">
         <v>6</v>
       </c>
-      <c r="E7" s="28"/>
-      <c r="F7" s="29"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="H7" s="41"/>
+      <c r="I7" s="42"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="13">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="13">
         <v>8</v>
       </c>
-      <c r="E8" s="30"/>
-      <c r="F8" s="31"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="H8" s="43"/>
+      <c r="I8" s="44"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>9</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="13">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="13">
         <v>10</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="H9" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="27"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="I9" s="40"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>11</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="13">
+        <v>42</v>
+      </c>
+      <c r="D10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="13">
         <v>12</v>
       </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="31"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="H10" s="43"/>
+      <c r="I10" s="44"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>13</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="13">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="13">
         <v>14</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="H11" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="27"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="I11" s="40"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>15</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="13">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
+        <v>102</v>
+      </c>
+      <c r="E12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="13">
         <v>16</v>
       </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="31"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="H12" s="43"/>
+      <c r="I12" s="44"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>17</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="13">
+        <v>46</v>
+      </c>
+      <c r="D13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" s="13">
         <v>18</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="H13" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="27"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="I13" s="40"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>19</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="13">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
+        <v>104</v>
+      </c>
+      <c r="E14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="13">
         <v>20</v>
       </c>
-      <c r="E14" s="30"/>
-      <c r="F14" s="31"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="H14" s="43"/>
+      <c r="I14" s="44"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>21</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="13">
+        <v>48</v>
+      </c>
+      <c r="D15" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" s="13">
         <v>22</v>
       </c>
-      <c r="E15" s="40" t="s">
+      <c r="H15" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="41"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="I15" s="46"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>23</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="13">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" t="s">
+        <v>67</v>
+      </c>
+      <c r="G16" s="13">
         <v>24</v>
       </c>
-      <c r="E16" s="42"/>
-      <c r="F16" s="43"/>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="H16" s="47"/>
+      <c r="I16" s="48"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <v>25</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="13">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>107</v>
+      </c>
+      <c r="E17" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="13">
         <v>26</v>
       </c>
-      <c r="E17" s="44" t="s">
+      <c r="H17" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="45"/>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="I17" s="50"/>
+      <c r="J17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>27</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="13">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18" t="s">
+        <v>69</v>
+      </c>
+      <c r="G18" s="13">
         <v>28</v>
       </c>
-      <c r="E18" s="44" t="s">
+      <c r="H18" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="45"/>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="I18" s="50"/>
+      <c r="J18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <v>29</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="13">
+        <v>36</v>
+      </c>
+      <c r="D19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19" t="s">
+        <v>70</v>
+      </c>
+      <c r="G19" s="13">
         <v>30</v>
       </c>
-      <c r="E19" s="21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="H19" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="J19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>31</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="13">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
+        <v>110</v>
+      </c>
+      <c r="E20" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" s="13">
         <v>32</v>
       </c>
-      <c r="E20" s="21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="H20" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="J20" t="s">
+        <v>114</v>
+      </c>
+      <c r="K20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>33</v>
       </c>
       <c r="B21" s="22"/>
-      <c r="D21" s="13">
+      <c r="D21" t="s">
+        <v>111</v>
+      </c>
+      <c r="E21" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" s="13">
         <v>34</v>
       </c>
-      <c r="E21" s="14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="H21" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="J21" t="s">
+        <v>115</v>
+      </c>
+      <c r="K21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>35</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="13">
+        <v>49</v>
+      </c>
+      <c r="D22" t="s">
+        <v>112</v>
+      </c>
+      <c r="E22" t="s">
+        <v>93</v>
+      </c>
+      <c r="G22" s="13">
         <v>36</v>
       </c>
-      <c r="E22" s="14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="H22" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="J22" t="s">
+        <v>117</v>
+      </c>
+      <c r="K22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <v>37</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="13">
+        <v>50</v>
+      </c>
+      <c r="D23" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" t="s">
+        <v>94</v>
+      </c>
+      <c r="G23" s="13">
         <v>38</v>
       </c>
-      <c r="E23" s="14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="H23" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="J23" t="s">
+        <v>118</v>
+      </c>
+      <c r="K23" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <v>39</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" s="13">
+        <v>33</v>
+      </c>
+      <c r="D24" t="s">
+        <v>98</v>
+      </c>
+      <c r="E24" t="s">
+        <v>73</v>
+      </c>
+      <c r="G24" s="13">
         <v>40</v>
       </c>
-      <c r="E24" s="15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="H24" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="J24" t="s">
+        <v>119</v>
+      </c>
+      <c r="K24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <v>41</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="25"/>
-      <c r="D25" s="13">
+      <c r="C25" s="29"/>
+      <c r="G25" s="13">
         <v>42</v>
       </c>
-      <c r="E25" s="16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="H25" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J25" t="s">
+        <v>120</v>
+      </c>
+      <c r="K25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>43</v>
       </c>
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="37"/>
-      <c r="D26" s="13">
+      <c r="C26" s="33"/>
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
+        <v>77</v>
+      </c>
+      <c r="G26" s="13">
         <v>44</v>
       </c>
-      <c r="E26" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
+      <c r="H26" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="I26" s="56"/>
+      <c r="J26" t="s">
+        <v>121</v>
+      </c>
+      <c r="K26" s="56" t="s">
+        <v>87</v>
+      </c>
       <c r="L26" s="12"/>
       <c r="M26" s="12"/>
       <c r="N26" s="12"/>
@@ -1340,43 +1701,59 @@
       <c r="V26" s="12"/>
       <c r="W26" s="12"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>45</v>
       </c>
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="37"/>
-      <c r="D27" s="13">
+      <c r="C27" s="33"/>
+      <c r="D27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="13">
         <v>46</v>
       </c>
-      <c r="E27" s="15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="H27" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="J27" t="s">
+        <v>122</v>
+      </c>
+      <c r="K27" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>47</v>
       </c>
-      <c r="B28" s="36" t="s">
+      <c r="B28" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="37"/>
-      <c r="D28" s="13">
+      <c r="C28" s="33"/>
+      <c r="D28" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" t="s">
+        <v>74</v>
+      </c>
+      <c r="G28" s="13">
         <v>48</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="H28" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F28" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
+      <c r="I28" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="J28" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="K28" s="56" t="s">
+        <v>89</v>
+      </c>
       <c r="L28" s="12"/>
       <c r="M28" s="12"/>
       <c r="N28" s="12"/>
@@ -1390,88 +1767,130 @@
       <c r="V28" s="12"/>
       <c r="W28" s="12"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <v>49</v>
       </c>
-      <c r="B29" s="36" t="s">
+      <c r="B29" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="37"/>
-      <c r="D29" s="13">
+      <c r="C29" s="33"/>
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" t="s">
+        <v>75</v>
+      </c>
+      <c r="G29" s="13">
         <v>50</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="H29" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="I29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J29" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="K29" s="57" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>51</v>
       </c>
-      <c r="B30" s="36" t="s">
+      <c r="B30" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="37"/>
-      <c r="D30" s="13">
+      <c r="C30" s="33"/>
+      <c r="D30" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" t="s">
+        <v>76</v>
+      </c>
+      <c r="G30" s="13">
         <v>52</v>
       </c>
-      <c r="E30" s="21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="H30" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="J30" s="57" t="s">
+        <v>123</v>
+      </c>
+      <c r="K30" s="56" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
         <v>53</v>
       </c>
-      <c r="B31" s="36" t="s">
+      <c r="B31" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="37"/>
-      <c r="D31" s="13">
+      <c r="C31" s="33"/>
+      <c r="D31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" t="s">
+        <v>78</v>
+      </c>
+      <c r="G31" s="13">
         <v>54</v>
       </c>
-      <c r="E31" s="24" t="s">
+      <c r="H31" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="F31" s="25"/>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="I31" s="38"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
         <v>55</v>
       </c>
-      <c r="B32" s="36" t="s">
+      <c r="B32" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="37"/>
-      <c r="D32" s="13">
+      <c r="C32" s="33"/>
+      <c r="D32" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" t="s">
+        <v>79</v>
+      </c>
+      <c r="G32" s="13">
         <v>56</v>
       </c>
-      <c r="E32" s="32" t="s">
+      <c r="H32" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="F32" s="33"/>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="I32" s="52"/>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
         <v>57</v>
       </c>
-      <c r="B33" s="36" t="s">
+      <c r="B33" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="37"/>
-      <c r="D33" s="13">
+      <c r="C33" s="33"/>
+      <c r="D33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" t="s">
+        <v>92</v>
+      </c>
+      <c r="G33" s="13">
         <v>58</v>
       </c>
-      <c r="E33" s="32" t="s">
+      <c r="H33" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="F33" s="33"/>
-    </row>
-    <row r="34" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I33" s="52"/>
+    </row>
+    <row r="34" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="19">
         <v>59</v>
       </c>
@@ -1479,16 +1898,15 @@
         <v>2</v>
       </c>
       <c r="C34" s="35"/>
-      <c r="D34" s="19">
+      <c r="G34" s="19">
         <v>60</v>
       </c>
-      <c r="E34" s="34" t="s">
+      <c r="H34" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="F34" s="35"/>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="D45" s="12"/>
+      <c r="I34" s="54"/>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
@@ -1509,8 +1927,7 @@
       <c r="V45" s="12"/>
       <c r="W45" s="12"/>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="D47" s="12"/>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="E47" s="12"/>
       <c r="F47" s="12"/>
       <c r="G47" s="12"/>
@@ -1531,8 +1948,7 @@
       <c r="V47" s="12"/>
       <c r="W47" s="12"/>
     </row>
-    <row r="49" spans="4:23" x14ac:dyDescent="0.35">
-      <c r="D49" s="12"/>
+    <row r="49" spans="4:23" x14ac:dyDescent="0.25">
       <c r="E49" s="12"/>
       <c r="F49" s="12"/>
       <c r="G49" s="12"/>
@@ -1553,7 +1969,7 @@
       <c r="V49" s="12"/>
       <c r="W49" s="12"/>
     </row>
-    <row r="51" spans="4:23" x14ac:dyDescent="0.35">
+    <row r="51" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D51" s="12"/>
       <c r="E51" s="12"/>
       <c r="F51" s="12"/>
@@ -1575,7 +1991,7 @@
       <c r="V51" s="12"/>
       <c r="W51" s="12"/>
     </row>
-    <row r="53" spans="4:23" x14ac:dyDescent="0.35">
+    <row r="53" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D53" s="12"/>
       <c r="E53" s="12"/>
       <c r="F53" s="12"/>
@@ -1597,7 +2013,7 @@
       <c r="V53" s="12"/>
       <c r="W53" s="12"/>
     </row>
-    <row r="55" spans="4:23" x14ac:dyDescent="0.35">
+    <row r="55" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D55" s="12"/>
       <c r="E55" s="12"/>
       <c r="F55" s="12"/>
@@ -1619,7 +2035,7 @@
       <c r="V55" s="12"/>
       <c r="W55" s="12"/>
     </row>
-    <row r="57" spans="4:23" x14ac:dyDescent="0.35">
+    <row r="57" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D57" s="12"/>
       <c r="E57" s="12"/>
       <c r="F57" s="12"/>
@@ -1641,7 +2057,7 @@
       <c r="V57" s="12"/>
       <c r="W57" s="12"/>
     </row>
-    <row r="58" spans="4:23" x14ac:dyDescent="0.35">
+    <row r="58" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D58" s="12"/>
       <c r="E58" s="12"/>
       <c r="F58" s="12"/>
@@ -1663,7 +2079,7 @@
       <c r="V58" s="12"/>
       <c r="W58" s="12"/>
     </row>
-    <row r="59" spans="4:23" x14ac:dyDescent="0.35">
+    <row r="59" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D59" s="12"/>
       <c r="E59" s="12"/>
       <c r="F59" s="12"/>
@@ -1685,7 +2101,7 @@
       <c r="V59" s="12"/>
       <c r="W59" s="12"/>
     </row>
-    <row r="61" spans="4:23" x14ac:dyDescent="0.35">
+    <row r="61" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D61" s="12"/>
       <c r="E61" s="12"/>
       <c r="F61" s="12"/>
@@ -1707,7 +2123,7 @@
       <c r="V61" s="12"/>
       <c r="W61" s="12"/>
     </row>
-    <row r="63" spans="4:23" x14ac:dyDescent="0.35">
+    <row r="63" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D63" s="12"/>
       <c r="E63" s="12"/>
       <c r="F63" s="12"/>
@@ -1729,7 +2145,7 @@
       <c r="V63" s="12"/>
       <c r="W63" s="12"/>
     </row>
-    <row r="64" spans="4:23" x14ac:dyDescent="0.35">
+    <row r="64" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D64" s="12"/>
       <c r="E64" s="12"/>
       <c r="F64" s="12"/>
@@ -1752,32 +2168,19 @@
       <c r="W64" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="12">
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B31:C31"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E15:F16"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B26:C26"/>
-    <mergeCell ref="E13:F14"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F8"/>
-    <mergeCell ref="E9:F10"/>
-    <mergeCell ref="E11:F12"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
working on the routing
</commit_message>
<xml_diff>
--- a/Pinout.xlsx
+++ b/Pinout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nico\Desktop\PSoM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B5FE9D-8B69-4169-AF56-240FC6BFDAF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C65626E-CE28-4403-B840-BEE069FD8FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30720" yWindow="-11292" windowWidth="25920" windowHeight="13524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9520" yWindow="900" windowWidth="9750" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -711,7 +711,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -776,10 +776,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -788,19 +794,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1083,21 +1082,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
@@ -1133,8 +1132,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="24" t="s">
         <v>0</v>
       </c>
@@ -1166,14 +1165,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" s="13">
         <v>1</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="49"/>
+      <c r="C5" s="47"/>
       <c r="G5" s="13">
         <v>2</v>
       </c>
@@ -1196,14 +1195,14 @@
       <c r="V5" s="12"/>
       <c r="W5" s="12"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" s="13">
         <v>3</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="51"/>
+      <c r="C6" s="45"/>
       <c r="G6" s="13">
         <v>4</v>
       </c>
@@ -1226,7 +1225,7 @@
       <c r="V6" s="12"/>
       <c r="W6" s="12"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" s="13">
         <v>5</v>
       </c>
@@ -1245,7 +1244,7 @@
       <c r="H7" s="32"/>
       <c r="I7" s="33"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" s="13">
         <v>7</v>
       </c>
@@ -1264,7 +1263,7 @@
       <c r="H8" s="34"/>
       <c r="I8" s="35"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" s="13">
         <v>9</v>
       </c>
@@ -1285,7 +1284,7 @@
       </c>
       <c r="I9" s="31"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" s="13">
         <v>11</v>
       </c>
@@ -1304,7 +1303,7 @@
       <c r="H10" s="34"/>
       <c r="I10" s="35"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" s="13">
         <v>13</v>
       </c>
@@ -1325,7 +1324,7 @@
       </c>
       <c r="I11" s="31"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" s="13">
         <v>15</v>
       </c>
@@ -1344,7 +1343,7 @@
       <c r="H12" s="34"/>
       <c r="I12" s="35"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13" s="13">
         <v>17</v>
       </c>
@@ -1368,7 +1367,7 @@
       </c>
       <c r="I13" s="31"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" s="13">
         <v>19</v>
       </c>
@@ -1390,7 +1389,7 @@
       <c r="H14" s="34"/>
       <c r="I14" s="35"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" s="13">
         <v>21</v>
       </c>
@@ -1414,7 +1413,7 @@
       </c>
       <c r="I15" s="37"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" s="13">
         <v>23</v>
       </c>
@@ -1433,7 +1432,7 @@
       <c r="H16" s="38"/>
       <c r="I16" s="39"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A17" s="13">
         <v>25</v>
       </c>
@@ -1457,7 +1456,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18" s="13">
         <v>27</v>
       </c>
@@ -1481,7 +1480,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A19" s="13">
         <v>29</v>
       </c>
@@ -1507,7 +1506,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20" s="13">
         <v>31</v>
       </c>
@@ -1533,7 +1532,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21" s="13">
         <v>33</v>
       </c>
@@ -1550,7 +1549,7 @@
       <c r="H21" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="I21" s="52" t="s">
+      <c r="I21" t="s">
         <v>124</v>
       </c>
       <c r="J21" t="s">
@@ -1560,7 +1559,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A22" s="13">
         <v>35</v>
       </c>
@@ -1571,7 +1570,7 @@
         <v>112</v>
       </c>
       <c r="E22" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G22" s="13">
         <v>36</v>
@@ -1579,7 +1578,7 @@
       <c r="H22" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="I22" s="52" t="s">
+      <c r="I22" t="s">
         <v>125</v>
       </c>
       <c r="J22" t="s">
@@ -1589,7 +1588,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A23" s="13">
         <v>37</v>
       </c>
@@ -1600,7 +1599,7 @@
         <v>97</v>
       </c>
       <c r="E23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G23" s="13">
         <v>38</v>
@@ -1615,7 +1614,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24" s="13">
         <v>39</v>
       </c>
@@ -1641,14 +1640,14 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A25" s="13">
         <v>41</v>
       </c>
-      <c r="B25" s="48" t="s">
+      <c r="B25" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="49"/>
+      <c r="C25" s="47"/>
       <c r="G25" s="13">
         <v>42</v>
       </c>
@@ -1662,14 +1661,14 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A26" s="13">
         <v>43</v>
       </c>
-      <c r="B26" s="46" t="s">
+      <c r="B26" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="47"/>
+      <c r="C26" s="49"/>
       <c r="D26" t="s">
         <v>7</v>
       </c>
@@ -1702,14 +1701,14 @@
       <c r="V26" s="12"/>
       <c r="W26" s="12"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A27" s="13">
         <v>45</v>
       </c>
-      <c r="B27" s="46" t="s">
+      <c r="B27" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="47"/>
+      <c r="C27" s="49"/>
       <c r="D27" t="s">
         <v>8</v>
       </c>
@@ -1726,14 +1725,14 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A28" s="13">
         <v>47</v>
       </c>
-      <c r="B28" s="46" t="s">
+      <c r="B28" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="47"/>
+      <c r="C28" s="49"/>
       <c r="D28" s="12" t="s">
         <v>9</v>
       </c>
@@ -1768,14 +1767,14 @@
       <c r="V28" s="12"/>
       <c r="W28" s="12"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A29" s="13">
         <v>49</v>
       </c>
-      <c r="B29" s="46" t="s">
+      <c r="B29" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="47"/>
+      <c r="C29" s="49"/>
       <c r="D29" t="s">
         <v>10</v>
       </c>
@@ -1798,14 +1797,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A30" s="13">
         <v>51</v>
       </c>
-      <c r="B30" s="46" t="s">
+      <c r="B30" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="47"/>
+      <c r="C30" s="49"/>
       <c r="D30" s="12" t="s">
         <v>11</v>
       </c>
@@ -1825,14 +1824,14 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A31" s="13">
         <v>53</v>
       </c>
-      <c r="B31" s="46" t="s">
+      <c r="B31" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="47"/>
+      <c r="C31" s="49"/>
       <c r="D31" t="s">
         <v>12</v>
       </c>
@@ -1847,14 +1846,14 @@
       </c>
       <c r="I31" s="29"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A32" s="13">
         <v>55</v>
       </c>
-      <c r="B32" s="46" t="s">
+      <c r="B32" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="47"/>
+      <c r="C32" s="49"/>
       <c r="D32" s="12" t="s">
         <v>13</v>
       </c>
@@ -1869,14 +1868,14 @@
       </c>
       <c r="I32" s="40"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A33" s="13">
         <v>57</v>
       </c>
-      <c r="B33" s="46" t="s">
+      <c r="B33" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="47"/>
+      <c r="C33" s="49"/>
       <c r="D33" t="s">
         <v>14</v>
       </c>
@@ -1891,14 +1890,14 @@
       </c>
       <c r="I33" s="40"/>
     </row>
-    <row r="34" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="19">
         <v>59</v>
       </c>
-      <c r="B34" s="44" t="s">
+      <c r="B34" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C34" s="45"/>
+      <c r="C34" s="51"/>
       <c r="G34" s="19">
         <v>60</v>
       </c>
@@ -1907,7 +1906,7 @@
       </c>
       <c r="I34" s="42"/>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
@@ -1928,7 +1927,7 @@
       <c r="V45" s="12"/>
       <c r="W45" s="12"/>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
       <c r="E47" s="12"/>
       <c r="F47" s="12"/>
       <c r="G47" s="12"/>
@@ -1949,7 +1948,7 @@
       <c r="V47" s="12"/>
       <c r="W47" s="12"/>
     </row>
-    <row r="49" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:23" x14ac:dyDescent="0.35">
       <c r="E49" s="12"/>
       <c r="F49" s="12"/>
       <c r="G49" s="12"/>
@@ -1970,7 +1969,7 @@
       <c r="V49" s="12"/>
       <c r="W49" s="12"/>
     </row>
-    <row r="51" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:23" x14ac:dyDescent="0.35">
       <c r="D51" s="12"/>
       <c r="E51" s="12"/>
       <c r="F51" s="12"/>
@@ -1992,7 +1991,7 @@
       <c r="V51" s="12"/>
       <c r="W51" s="12"/>
     </row>
-    <row r="53" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:23" x14ac:dyDescent="0.35">
       <c r="D53" s="12"/>
       <c r="E53" s="12"/>
       <c r="F53" s="12"/>
@@ -2014,7 +2013,7 @@
       <c r="V53" s="12"/>
       <c r="W53" s="12"/>
     </row>
-    <row r="55" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:23" x14ac:dyDescent="0.35">
       <c r="D55" s="12"/>
       <c r="E55" s="12"/>
       <c r="F55" s="12"/>
@@ -2036,7 +2035,7 @@
       <c r="V55" s="12"/>
       <c r="W55" s="12"/>
     </row>
-    <row r="57" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:23" x14ac:dyDescent="0.35">
       <c r="D57" s="12"/>
       <c r="E57" s="12"/>
       <c r="F57" s="12"/>
@@ -2058,7 +2057,7 @@
       <c r="V57" s="12"/>
       <c r="W57" s="12"/>
     </row>
-    <row r="58" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:23" x14ac:dyDescent="0.35">
       <c r="D58" s="12"/>
       <c r="E58" s="12"/>
       <c r="F58" s="12"/>
@@ -2080,7 +2079,7 @@
       <c r="V58" s="12"/>
       <c r="W58" s="12"/>
     </row>
-    <row r="59" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:23" x14ac:dyDescent="0.35">
       <c r="D59" s="12"/>
       <c r="E59" s="12"/>
       <c r="F59" s="12"/>
@@ -2102,7 +2101,7 @@
       <c r="V59" s="12"/>
       <c r="W59" s="12"/>
     </row>
-    <row r="61" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:23" x14ac:dyDescent="0.35">
       <c r="D61" s="12"/>
       <c r="E61" s="12"/>
       <c r="F61" s="12"/>
@@ -2124,7 +2123,7 @@
       <c r="V61" s="12"/>
       <c r="W61" s="12"/>
     </row>
-    <row r="63" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:23" x14ac:dyDescent="0.35">
       <c r="D63" s="12"/>
       <c r="E63" s="12"/>
       <c r="F63" s="12"/>
@@ -2146,7 +2145,7 @@
       <c r="V63" s="12"/>
       <c r="W63" s="12"/>
     </row>
-    <row r="64" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:23" x14ac:dyDescent="0.35">
       <c r="D64" s="12"/>
       <c r="E64" s="12"/>
       <c r="F64" s="12"/>
@@ -2170,6 +2169,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B25:C25"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B30:C30"/>
@@ -2177,11 +2181,6 @@
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B25:C25"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>